<commit_message>
progress on estimation, need to correct stochastic singularity
</commit_message>
<xml_diff>
--- a/writeups/draft_to_dos.xlsx
+++ b/writeups/draft_to_dos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="1160" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>DRAFT TO DO'S</t>
   </si>
@@ -40,6 +40,48 @@
   </si>
   <si>
     <t>more discussion of the realtionship of the optimal policy function to the TR</t>
+  </si>
+  <si>
+    <t>write out target criterion, expanding the terms so the signs become clear</t>
+  </si>
+  <si>
+    <t>mapping from Kalman gain to k_t --&gt; compare estimation to evolution of Kalman gain</t>
+  </si>
+  <si>
+    <t>Gaetano Gaballo meeting, 11 June 2020, Notes 12, p 35</t>
+  </si>
+  <si>
+    <t>graph to understand the target criterion</t>
+  </si>
+  <si>
+    <t>two-period problem version of model w/ an intertemporal price people learn about, use it to show the mistake the CB makes when it assumes RE</t>
+  </si>
+  <si>
+    <t>Gaetano's selling points:</t>
+  </si>
+  <si>
+    <t>3. so how costly is it to assume plain vanilla rational expectations in short run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recall that discretion=commitment w/o RE </t>
+  </si>
+  <si>
+    <t>But how you depart from RE matters for how policy should deal with this fact. So I do 3 things</t>
+  </si>
+  <si>
+    <t>2. solve for optimal policy</t>
+  </si>
+  <si>
+    <t>3. tell you what mistake CB makes when it instead assumes RE</t>
+  </si>
+  <si>
+    <t>1. RE (a la Lucas) is great in long-run (don't fight RE!)</t>
+  </si>
+  <si>
+    <t>1. estimate an adaptive learning model (small departures from RE can match empirical facts --&gt; see how Marcet-Adam, Eusepi-Preston sell their models!)</t>
+  </si>
+  <si>
+    <t>2. but crisis has shown that things move quickly --&gt; you'd need large changes in the model to match drifting long-run expectations</t>
   </si>
 </sst>
 </file>
@@ -52,6 +94,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -422,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -464,6 +507,74 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
now the Taylor rule results are like meh
</commit_message>
<xml_diff>
--- a/writeups/draft_to_dos.xlsx
+++ b/writeups/draft_to_dos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>DRAFT TO DO'S</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Ryan meeting 5 June 2020, Notes 12, p. 20</t>
   </si>
   <si>
-    <t>more discussion of the realtionship of the optimal policy function to the TR</t>
-  </si>
-  <si>
     <t>write out target criterion, expanding the terms so the signs become clear</t>
   </si>
   <si>
@@ -82,6 +79,15 @@
   </si>
   <si>
     <t>2. but crisis has shown that things move quickly --&gt; you'd need large changes in the model to match drifting long-run expectations</t>
+  </si>
+  <si>
+    <t>more discussion of the relationship of the optimal policy function to the TR</t>
+  </si>
+  <si>
+    <t>see loss for RE-optimal TR coefficients under learning</t>
+  </si>
+  <si>
+    <t>what is truly my message? Once I know, what would I want a paper to do to convince me of this message?</t>
   </si>
 </sst>
 </file>
@@ -94,7 +100,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -465,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -504,75 +509,85 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
still not quite good
</commit_message>
<xml_diff>
--- a/writeups/draft_to_dos.xlsx
+++ b/writeups/draft_to_dos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>DRAFT TO DO'S</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>what is truly my message? Once I know, what would I want a paper to do to convince me of this message?</t>
+  </si>
+  <si>
+    <t>read up on and have a stance to the flattening of the PC literature</t>
   </si>
 </sst>
 </file>
@@ -111,12 +114,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,12 +140,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -470,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -500,7 +512,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -576,7 +588,7 @@
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -586,8 +598,13 @@
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
still unidentified - gotta check procedures tomorra
</commit_message>
<xml_diff>
--- a/writeups/draft_to_dos.xlsx
+++ b/writeups/draft_to_dos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>DRAFT TO DO'S</t>
   </si>
@@ -91,13 +91,34 @@
   </si>
   <si>
     <t>read up on and have a stance to the flattening of the PC literature</t>
+  </si>
+  <si>
+    <t>get estimation identified</t>
+  </si>
+  <si>
+    <t>redo PEA-VFI: figures, interpretations</t>
+  </si>
+  <si>
+    <t>redo optimal Taylor rule: figures, table, interpretations</t>
+  </si>
+  <si>
+    <t>redo IRFs of model in app, possibly interpretations</t>
+  </si>
+  <si>
+    <t>App alternative specifications of anchoring function</t>
+  </si>
+  <si>
+    <t>App estimation procedure</t>
+  </si>
+  <si>
+    <t>do a welfare bit that compares welfare under the optimal policy, an optimal TR under anchoring and an optimal TR under RE (may not make it into first draft)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +132,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -140,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -149,6 +177,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -482,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -504,7 +535,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="30">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -525,7 +556,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -605,6 +636,41 @@
     <row r="21" spans="1:1">
       <c r="A21" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial VAR estimation too good?
</commit_message>
<xml_diff>
--- a/writeups/draft_to_dos.xlsx
+++ b/writeups/draft_to_dos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>DRAFT TO DO'S</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Incorporate in the optimal Taylor rule section an explanation of why time-invariant TR coefficients make sense. The reason is that the advantage of the TR is that it's simple to compute and to verify. Having time-varying coefficients undoes that simplicity.</t>
   </si>
   <si>
-    <t>Susanto's liquidity premium correction for TIPS inflation expectations</t>
-  </si>
-  <si>
     <t>See</t>
   </si>
   <si>
@@ -93,15 +90,6 @@
     <t>read up on and have a stance to the flattening of the PC literature</t>
   </si>
   <si>
-    <t>get estimation identified</t>
-  </si>
-  <si>
-    <t>redo PEA-VFI: figures, interpretations</t>
-  </si>
-  <si>
-    <t>redo optimal Taylor rule: figures, table, interpretations</t>
-  </si>
-  <si>
     <t>redo IRFs of model in app, possibly interpretations</t>
   </si>
   <si>
@@ -112,6 +100,21 @@
   </si>
   <si>
     <t>do a welfare bit that compares welfare under the optimal policy, an optimal TR under anchoring and an optimal TR under RE (may not make it into first draft)</t>
+  </si>
+  <si>
+    <t>redo PEA-VFI: figures, interpretations: di/dk, di/dpibar, Obs TR vs anch, PEA vs VFI X1 and X2</t>
+  </si>
+  <si>
+    <t>redo optimal Taylor rule: figures, table, interpretations: CB loss as a function of psi_pi in RE vs anchoring</t>
+  </si>
+  <si>
+    <t>get estimation identified: fig alpha hat, autocovariogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monpol should respond to expectations directly: raise int by x when expectations unanchor, which they do for y forecast errors. </t>
+  </si>
+  <si>
+    <t>Susanto's liquidity premium correction for TIPS inflation expectations (write up Notes 27 July and include VIX figure and Andreasen results) - done!</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -168,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,6 +189,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -516,7 +528,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -531,7 +543,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30">
@@ -539,138 +551,141 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
+      <c r="A4" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="3" t="s">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="3" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="1" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated figures with the Materials 37 candidate Mean(alph) = (0.3509;0.1427;0.0180;0.0005;0.0204;0.1406;0.3411)
</commit_message>
<xml_diff>
--- a/writeups/draft_to_dos.xlsx
+++ b/writeups/draft_to_dos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>DRAFT TO DO'S</t>
   </si>
@@ -90,9 +90,6 @@
     <t>read up on and have a stance to the flattening of the PC literature</t>
   </si>
   <si>
-    <t>redo IRFs of model in app, possibly interpretations</t>
-  </si>
-  <si>
     <t>App alternative specifications of anchoring function</t>
   </si>
   <si>
@@ -115,13 +112,22 @@
   </si>
   <si>
     <t>Susanto's liquidity premium correction for TIPS inflation expectations (write up Notes 27 July and include VIX figure and Andreasen results) - done!</t>
+  </si>
+  <si>
+    <t>redo IRFs of model in app, possibly interpretations - I decided to keep the old IRFs b/c they are better for interpretation</t>
+  </si>
+  <si>
+    <t>using materials 37 material right now</t>
+  </si>
+  <si>
+    <t>edit discussion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +148,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -174,8 +196,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -195,7 +219,9 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -528,7 +554,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -556,7 +582,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -645,7 +671,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -655,41 +681,48 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>23</v>
+      <c r="A29" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
completed the july draft for ZEW application
</commit_message>
<xml_diff>
--- a/writeups/draft_to_dos.xlsx
+++ b/writeups/draft_to_dos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>DRAFT TO DO'S</t>
   </si>
@@ -120,7 +120,13 @@
     <t>using materials 37 material right now</t>
   </si>
   <si>
-    <t>edit discussion</t>
+    <t>working on it with new sim_learnLH_pea_optimal.m</t>
+  </si>
+  <si>
+    <t>Note: objective_CB_approx.m should use the learning code …univariate.m, but there's a problem there, so I don't do that yet. 30 July 2020</t>
+  </si>
+  <si>
+    <t>need a number there too</t>
   </si>
 </sst>
 </file>
@@ -551,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -701,14 +707,14 @@
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="4" t="s">
@@ -718,6 +724,14 @@
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did first-pass calibration and redid PEA, VFI and Taylor-rule loss functions given it
</commit_message>
<xml_diff>
--- a/writeups/draft_to_dos.xlsx
+++ b/writeups/draft_to_dos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>DRAFT TO DO'S</t>
   </si>
@@ -117,9 +117,6 @@
     <t>redo IRFs of model in app, possibly interpretations - I decided to keep the old IRFs b/c they are better for interpretation</t>
   </si>
   <si>
-    <t>using materials 37 material right now</t>
-  </si>
-  <si>
     <t>working on it with new sim_learnLH_pea_optimal.m</t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>need a number there too</t>
+  </si>
+  <si>
+    <t>using materials 42 (23 August 2020 calibration) material right now</t>
+  </si>
+  <si>
+    <t>couldn't redo this, need to fix! So July 30 figures there</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -700,20 +703,23 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -726,12 +732,12 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>